<commit_message>
AmExpert credit dataset + uropean Cardholders Dataset.
</commit_message>
<xml_diff>
--- a/Merged dataset (missing).xlsx
+++ b/Merged dataset (missing).xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\imputation-show codes\兩credit (老師）\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\imputation-show codes\兩credit (老師）\Merged datasets\Merged-credit-datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C2701F-2365-4BAE-AD3B-EB5DB5F89CE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE1B569-FE76-4F75-9457-5F4C4C569889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -499,7 +499,7 @@
   <dimension ref="A1:AU1364"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
@@ -7674,7 +7674,7 @@
         <v>7.18</v>
       </c>
       <c r="AU75" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:47" x14ac:dyDescent="0.55000000000000004">
@@ -7769,7 +7769,7 @@
         <v>2</v>
       </c>
       <c r="AU76" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:47" x14ac:dyDescent="0.55000000000000004">
@@ -7864,7 +7864,7 @@
         <v>1</v>
       </c>
       <c r="AU77" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:47" x14ac:dyDescent="0.55000000000000004">
@@ -7959,7 +7959,7 @@
         <v>130.21</v>
       </c>
       <c r="AU78" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:47" x14ac:dyDescent="0.55000000000000004">
@@ -8054,7 +8054,7 @@
         <v>727.91</v>
       </c>
       <c r="AU79" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:47" x14ac:dyDescent="0.55000000000000004">
@@ -8149,7 +8149,7 @@
         <v>320.01</v>
       </c>
       <c r="AU80" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:47" x14ac:dyDescent="0.55000000000000004">
@@ -8244,7 +8244,7 @@
         <v>1.18</v>
       </c>
       <c r="AU81" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:47" x14ac:dyDescent="0.55000000000000004">
@@ -8339,7 +8339,7 @@
         <v>0</v>
       </c>
       <c r="AU82" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:47" x14ac:dyDescent="0.55000000000000004">
@@ -8434,7 +8434,7 @@
         <v>0.76</v>
       </c>
       <c r="AU83" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:47" x14ac:dyDescent="0.55000000000000004">
@@ -8529,7 +8529,7 @@
         <v>122.68</v>
       </c>
       <c r="AU84" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:47" x14ac:dyDescent="0.55000000000000004">
@@ -8624,7 +8624,7 @@
         <v>17.39</v>
       </c>
       <c r="AU85" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:47" x14ac:dyDescent="0.55000000000000004">
@@ -8719,7 +8719,7 @@
         <v>237.26</v>
       </c>
       <c r="AU86" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:47" x14ac:dyDescent="0.55000000000000004">
@@ -8814,7 +8814,7 @@
         <v>1</v>
       </c>
       <c r="AU87" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:47" x14ac:dyDescent="0.55000000000000004">
@@ -8909,7 +8909,7 @@
         <v>1096.99</v>
       </c>
       <c r="AU88" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:47" x14ac:dyDescent="0.55000000000000004">
@@ -9004,7 +9004,7 @@
         <v>7.59</v>
       </c>
       <c r="AU89" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:47" x14ac:dyDescent="0.55000000000000004">
@@ -9099,7 +9099,7 @@
         <v>0.77</v>
       </c>
       <c r="AU90" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:47" x14ac:dyDescent="0.55000000000000004">
@@ -9194,7 +9194,7 @@
         <v>390</v>
       </c>
       <c r="AU91" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:47" x14ac:dyDescent="0.55000000000000004">
@@ -30252,7 +30252,7 @@
         <v>0</v>
       </c>
       <c r="AU417" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="418" spans="31:47" x14ac:dyDescent="0.55000000000000004">
@@ -30305,7 +30305,7 @@
         <v>0</v>
       </c>
       <c r="AU418" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="419" spans="31:47" x14ac:dyDescent="0.55000000000000004">
@@ -30358,7 +30358,7 @@
         <v>1</v>
       </c>
       <c r="AU419" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="420" spans="31:47" x14ac:dyDescent="0.55000000000000004">
@@ -30411,7 +30411,7 @@
         <v>1</v>
       </c>
       <c r="AU420" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="421" spans="31:47" x14ac:dyDescent="0.55000000000000004">
@@ -30464,7 +30464,7 @@
         <v>0</v>
       </c>
       <c r="AU421" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="422" spans="31:47" x14ac:dyDescent="0.55000000000000004">
@@ -30517,7 +30517,7 @@
         <v>0</v>
       </c>
       <c r="AU422" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="423" spans="31:47" x14ac:dyDescent="0.55000000000000004">
@@ -30888,7 +30888,7 @@
         <v>1</v>
       </c>
       <c r="AU429" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="430" spans="31:47" x14ac:dyDescent="0.55000000000000004">
@@ -30941,7 +30941,7 @@
         <v>1</v>
       </c>
       <c r="AU430" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="431" spans="31:47" x14ac:dyDescent="0.55000000000000004">
@@ -30994,7 +30994,7 @@
         <v>1</v>
       </c>
       <c r="AU431" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="432" spans="31:47" x14ac:dyDescent="0.55000000000000004">
@@ -31153,7 +31153,7 @@
         <v>0</v>
       </c>
       <c r="AU434" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="435" spans="31:47" x14ac:dyDescent="0.55000000000000004">
@@ -31365,7 +31365,7 @@
         <v>1</v>
       </c>
       <c r="AU438" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="439" spans="31:47" x14ac:dyDescent="0.55000000000000004">
@@ -31418,7 +31418,7 @@
         <v>0</v>
       </c>
       <c r="AU439" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="440" spans="31:47" x14ac:dyDescent="0.55000000000000004">
@@ -52300,7 +52300,7 @@
         <v>0</v>
       </c>
       <c r="AU833" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="834" spans="31:47" x14ac:dyDescent="0.55000000000000004">
@@ -52353,7 +52353,7 @@
         <v>0</v>
       </c>
       <c r="AU834" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="835" spans="31:47" x14ac:dyDescent="0.55000000000000004">
@@ -52406,7 +52406,7 @@
         <v>1</v>
       </c>
       <c r="AU835" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="836" spans="31:47" x14ac:dyDescent="0.55000000000000004">
@@ -52459,7 +52459,7 @@
         <v>1</v>
       </c>
       <c r="AU836" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="837" spans="31:47" x14ac:dyDescent="0.55000000000000004">
@@ -52565,7 +52565,7 @@
         <v>1</v>
       </c>
       <c r="AU838" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="839" spans="31:47" x14ac:dyDescent="0.55000000000000004">
@@ -52830,7 +52830,7 @@
         <v>1</v>
       </c>
       <c r="AU843" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="844" spans="31:47" x14ac:dyDescent="0.55000000000000004">

</xml_diff>